<commit_message>
Last changes in results
Just the results from some institutions
</commit_message>
<xml_diff>
--- a/puntajes_COLEGIO LIBERTADOR SIMON BOLIVAR.xlsx
+++ b/puntajes_COLEGIO LIBERTADOR SIMON BOLIVAR.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">PUNT_INGLES</t>
   </si>
@@ -33,6 +33,33 @@
   </si>
   <si>
     <t xml:space="preserve">anno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20224</t>
   </si>
 </sst>
 </file>
@@ -387,6 +414,213 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.563802729587219</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.623444919300612</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.187241345191466</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.556921174267507</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.568495483749721</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.174031355808975</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.583980300283867</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.563204862663672</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.174891914482683</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.632302529661763</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.647221592890618</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.630732000949296</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.581557776624798</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.656122813055518</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.629169621555573</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.646653955492808</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.607579575705563</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.634231362238096</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.614170788750637</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.67237468396115</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.633209475958396</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.674809643379912</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.627964250593938</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.654438326783103</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.675006017427407</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.683088012664057</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.661253805060417</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.644665302001612</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.665297468910414</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.687720290565028</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.705730198925224</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.686346370402789</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.68307294526246</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.670839379294631</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.708803163884336</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.715436210207303</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.715972124701587</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.730728612044077</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.714127670138964</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.579830382431018</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.640953192347311</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.573012050964629</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.630758582131225</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.65695841816287</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.621913624096086</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>